<commit_message>
model/methods good enough to move forward
</commit_message>
<xml_diff>
--- a/GroupPolarizationStatmod/data/StudiesAnalysis.xlsx
+++ b/GroupPolarizationStatmod/data/StudiesAnalysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mt/workspace/gp-statmod/GroupPolarizationStatmod/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{A6EEC309-9D4E-9C45-91E0-02E561BB3BB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{570FD1DD-24F6-9E40-91A0-9B565515DA10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{28B24468-AC29-524C-88BB-DBB8559362C2}"/>
+    <workbookView xWindow="8400" yWindow="2400" windowWidth="21600" windowHeight="19200" xr2:uid="{28B24468-AC29-524C-88BB-DBB8559362C2}"/>
   </bookViews>
   <sheets>
     <sheet name="StudiesAnalysis" sheetId="1" r:id="rId1"/>
@@ -562,7 +562,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -760,6 +760,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -921,15 +927,17 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1324,18 +1332,21 @@
   <dimension ref="A1:U64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D63" sqref="D63"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" customWidth="1"/>
     <col min="3" max="3" width="17.33203125" customWidth="1"/>
     <col min="4" max="4" width="16.33203125" customWidth="1"/>
     <col min="5" max="5" width="17.83203125" customWidth="1"/>
     <col min="6" max="6" width="19.5" customWidth="1"/>
     <col min="7" max="7" width="14.6640625" customWidth="1"/>
     <col min="8" max="8" width="16.5" customWidth="1"/>
+    <col min="13" max="13" width="20.6640625" customWidth="1"/>
+    <col min="14" max="14" width="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -1781,68 +1792,68 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="8" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="8">
         <v>4.3214805470000002</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="8">
         <v>1.897926743</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="8">
         <v>-0.61</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="8">
         <v>-1.04</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="8">
         <v>-0.43</v>
       </c>
-      <c r="H8" t="s">
-        <v>23</v>
-      </c>
-      <c r="I8">
+      <c r="H8" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" s="8">
         <v>140</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="8">
         <v>-1.2</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="8">
         <v>0.05</v>
       </c>
-      <c r="L8" s="1">
+      <c r="L8" s="9">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="8">
         <v>5.7874900000000004E-4</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="8">
         <v>4.88679E-4</v>
       </c>
-      <c r="O8">
+      <c r="O8" s="8">
         <v>-3</v>
       </c>
-      <c r="P8">
+      <c r="P8" s="8">
         <v>3</v>
       </c>
-      <c r="Q8" t="b">
-        <v>1</v>
-      </c>
-      <c r="R8">
-        <v>1</v>
-      </c>
-      <c r="S8" t="b">
-        <v>1</v>
-      </c>
-      <c r="T8">
-        <v>1</v>
-      </c>
-      <c r="U8" t="s">
+      <c r="Q8" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="R8" s="8">
+        <v>1</v>
+      </c>
+      <c r="S8" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="T8" s="8">
+        <v>1</v>
+      </c>
+      <c r="U8" s="8" t="s">
         <v>33</v>
       </c>
     </row>
@@ -5244,5 +5255,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
calculating quantiles and writing analysis
</commit_message>
<xml_diff>
--- a/GroupPolarizationStatmod/data/StudiesAnalysis.xlsx
+++ b/GroupPolarizationStatmod/data/StudiesAnalysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mt/workspace/gp-statmod/GroupPolarizationStatmod/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{570FD1DD-24F6-9E40-91A0-9B565515DA10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E5D113EC-79AF-1547-A43A-1AC932A12AEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8400" yWindow="2400" windowWidth="21600" windowHeight="19200" xr2:uid="{28B24468-AC29-524C-88BB-DBB8559362C2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{28B24468-AC29-524C-88BB-DBB8559362C2}"/>
   </bookViews>
   <sheets>
     <sheet name="StudiesAnalysis" sheetId="1" r:id="rId1"/>
@@ -1331,8 +1331,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39A9D91A-08D2-B24C-9D0F-D8C217A4413A}">
   <dimension ref="A1:U64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="AA7" sqref="AA7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
nearly done with Analysis
</commit_message>
<xml_diff>
--- a/GroupPolarizationStatmod/data/StudiesAnalysis.xlsx
+++ b/GroupPolarizationStatmod/data/StudiesAnalysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mt/workspace/gp-statmod/GroupPolarizationStatmod/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E5D113EC-79AF-1547-A43A-1AC932A12AEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{41B4C351-E463-6E4C-8293-29208FEC3C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{28B24468-AC29-524C-88BB-DBB8559362C2}"/>
   </bookViews>
@@ -1331,8 +1331,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39A9D91A-08D2-B24C-9D0F-D8C217A4413A}">
   <dimension ref="A1:U64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="AA7" sqref="AA7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>